<commit_message>
fix done login admin user
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="82">
   <si>
     <t>Name</t>
   </si>
@@ -248,6 +248,18 @@
   </si>
   <si>
     <t>0962563090</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lê Thành Đạt </t>
+  </si>
+  <si>
+    <t>Inter</t>
+  </si>
+  <si>
+    <t>dat.lethanh2@ncc.asia</t>
+  </si>
+  <si>
+    <t>01 291</t>
   </si>
 </sst>
 </file>
@@ -255,9 +267,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="23">
@@ -303,6 +315,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
@@ -310,17 +330,17 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -343,39 +363,9 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -387,6 +377,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
@@ -403,30 +401,44 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -441,187 +453,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -635,17 +647,35 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </left>
       <right style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </right>
       <top style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -665,26 +695,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </right>
       <top style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -707,8 +728,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -723,29 +744,20 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -758,131 +770,131 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="22" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="21" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="21" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="15" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="8" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -898,6 +910,7 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="7" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" quotePrefix="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" quotePrefix="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" quotePrefix="1"/>
@@ -1222,8 +1235,8 @@
   <sheetPr/>
   <dimension ref="A1:E19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5" outlineLevelCol="4"/>
@@ -1415,7 +1428,7 @@
       <c r="C11" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="D11" s="9" t="s">
+      <c r="D11" s="10" t="s">
         <v>48</v>
       </c>
       <c r="E11" s="1" t="s">
@@ -1432,7 +1445,7 @@
       <c r="C12" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="D12" s="10" t="s">
+      <c r="D12" s="11" t="s">
         <v>53</v>
       </c>
       <c r="E12" s="1" t="s">
@@ -1483,7 +1496,7 @@
       <c r="C15" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="D15" s="10" t="s">
+      <c r="D15" s="11" t="s">
         <v>65</v>
       </c>
       <c r="E15" s="1" t="s">
@@ -1517,7 +1530,7 @@
       <c r="C17" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="D17" s="10" t="s">
+      <c r="D17" s="11" t="s">
         <v>73</v>
       </c>
       <c r="E17" s="1" t="s">
@@ -1534,7 +1547,7 @@
       <c r="C18" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="D18" s="11" t="s">
+      <c r="D18" s="12" t="s">
         <v>77</v>
       </c>
       <c r="E18" s="1" t="s">
@@ -1542,10 +1555,18 @@
       </c>
     </row>
     <row r="19" spans="1:5">
-      <c r="A19" s="8"/>
-      <c r="B19" s="8"/>
-      <c r="C19" s="8"/>
-      <c r="D19" s="8"/>
+      <c r="A19" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="B19" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="C19" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="D19" s="8" t="s">
+        <v>81</v>
+      </c>
       <c r="E19" s="8"/>
     </row>
   </sheetData>
@@ -1567,6 +1588,7 @@
     <hyperlink ref="C17" r:id="rId15" display="tien.nguyenhuu@ncc.asia"/>
     <hyperlink ref="C18" r:id="rId16" display="van.vu@ncc.asia"/>
     <hyperlink ref="C3" r:id="rId17" display="trung.dotrong@ncc.asia"/>
+    <hyperlink ref="C19" r:id="rId18" display="dat.lethanh2@ncc.asia"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>